<commit_message>
deleting irrelevant attributes in data model
</commit_message>
<xml_diff>
--- a/data_relations.xlsx
+++ b/data_relations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erka/workspace/formula1_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77634EB7-1AFB-5D4D-A365-A957DA68511A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9521B059-972A-9543-8C50-BDC51B1F19AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{0C26CD5C-2603-FD49-A2AA-583BACEE6CB9}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="1. Unsorted Data" sheetId="1" r:id="rId1"/>
     <sheet name="2. Combine Data" sheetId="2" r:id="rId2"/>
     <sheet name="3. Delete irrelevant Attributes" sheetId="3" r:id="rId3"/>
+    <sheet name="4. Renaming" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="59">
   <si>
     <t>year</t>
   </si>
@@ -735,7 +736,7 @@
   <dimension ref="B2:Z22"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF7CABD-B5C9-8B40-B600-4F6335FB1415}">
   <dimension ref="B2:Z22"/>
   <sheetViews>
-    <sheetView zoomScale="158" workbookViewId="0">
-      <selection activeCell="H20" sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1555,7 +1556,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2298,4 +2299,417 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF754FB6-D295-B240-9D90-205E5BCF9236}">
+  <dimension ref="A1:T22"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+    </row>
+    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="5"/>
+      <c r="T3" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" t="s">
+        <v>45</v>
+      </c>
+      <c r="T9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" t="s">
+        <v>40</v>
+      </c>
+      <c r="R10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="R11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="T12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="T13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="T14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="T15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="T16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="T17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="T18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="T19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="T20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="T21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>